<commit_message>
feat: reorganize project and commit README
</commit_message>
<xml_diff>
--- a/rustkg_be/sandbox/analyze/charts/analyze.xlsx
+++ b/rustkg_be/sandbox/analyze/charts/analyze.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dj\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lessons\projects\rustKG\rustkg_be\sandbox\analyze\charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA43A19A-6D95-4325-97D8-7D245F057F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9DBF5B-B457-4CD0-9EEF-E0444CEBE80F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="6756" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="diff_data" sheetId="1" r:id="rId1"/>
@@ -10058,6 +10058,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="291798080"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -28085,8 +28086,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="18932338" y="163131"/>
-          <a:ext cx="14124050" cy="8466524"/>
+          <a:off x="20246959" y="165671"/>
+          <a:ext cx="14099131" cy="8223268"/>
           <a:chOff x="16570817" y="163131"/>
           <a:chExt cx="12855441" cy="8391508"/>
         </a:xfrm>
@@ -28204,8 +28205,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="19117796" y="9617658"/>
-          <a:ext cx="14044391" cy="7172782"/>
+          <a:off x="20434511" y="9343510"/>
+          <a:ext cx="14016108" cy="6966836"/>
           <a:chOff x="16591725" y="9459008"/>
           <a:chExt cx="12753996" cy="7053046"/>
         </a:xfrm>
@@ -28359,8 +28360,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="18776063" y="55813835"/>
-          <a:ext cx="14095140" cy="8464795"/>
+          <a:off x="20089414" y="54226713"/>
+          <a:ext cx="14069397" cy="8221538"/>
           <a:chOff x="16570817" y="163131"/>
           <a:chExt cx="12855441" cy="8391508"/>
         </a:xfrm>
@@ -28478,8 +28479,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="18783928" y="64450606"/>
-          <a:ext cx="14044391" cy="7172783"/>
+          <a:off x="20098549" y="62613808"/>
+          <a:ext cx="14017378" cy="6966837"/>
           <a:chOff x="16591725" y="9459008"/>
           <a:chExt cx="12753996" cy="7053046"/>
         </a:xfrm>
@@ -28981,14 +28982,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD676"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A599" zoomScale="74" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="T609" sqref="T609"/>
+    <sheetView tabSelected="1" topLeftCell="A606" zoomScale="74" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A617" sqref="A617"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.4140625" customWidth="1"/>
+    <col min="2" max="2" width="36.1640625" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.58203125" bestFit="1" customWidth="1"/>
     <col min="6" max="11" width="9" bestFit="1" customWidth="1"/>
@@ -60518,7 +60519,7 @@
         <v>deepseek-r1-250120</v>
       </c>
       <c r="P618" t="str">
-        <f t="shared" ref="P618:P636" si="41">D618</f>
+        <f t="shared" ref="P618:P626" si="41">D618</f>
         <v>split</v>
       </c>
       <c r="Q618" cm="1">

</xml_diff>